<commit_message>
finalización diseño secciones 2 y 3
</commit_message>
<xml_diff>
--- a/app/tables/tabla_jacobi.xlsx
+++ b/app/tables/tabla_jacobi.xlsx
@@ -463,17 +463,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-2.0</t>
+          <t>1.8</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>0.857142857142857</t>
         </is>
       </c>
     </row>
@@ -485,17 +485,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>0.428571428571429</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>14.0</t>
+          <t>-0.428571428571428</t>
         </is>
       </c>
     </row>
@@ -507,17 +507,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1.11111111111111</t>
+          <t>1.77777777777778</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>-18.0</t>
+          <t>2.48571428571429</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>0.551020408163265</t>
         </is>
       </c>
     </row>
@@ -529,17 +529,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.666666666666667</t>
+          <t>1.70666666666667</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-12.6666666666667</t>
+          <t>0.918367346938776</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>30.0</t>
+          <t>-0.918367346938775</t>
         </is>
       </c>
     </row>
@@ -551,17 +551,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0.677966101694915</t>
+          <t>5.56521739130435</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>-39.3333333333333</t>
+          <t>3.26938775510204</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>24.6666666666667</t>
+          <t>0.201166180758017</t>
         </is>
       </c>
     </row>
@@ -573,17 +573,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0.519480519480519</t>
+          <t>1.21183431952663</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>-32.2222222222222</t>
+          <t>1.47813411078717</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>51.3333333333333</t>
+          <t>-1.47813411078717</t>
         </is>
       </c>
     </row>
@@ -595,17 +595,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0.524590163934426</t>
+          <t>6.44025157232704</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>-67.7777777777778</t>
+          <t>4.16501457725947</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>44.2222222222222</t>
+          <t>-0.198667221990837</t>
         </is>
       </c>
     </row>
@@ -617,17 +617,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0.445682451253482</t>
+          <t>0.966607669616519</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>-58.2962962962963</t>
+          <t>2.11786755518534</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>79.7777777777778</t>
+          <t>-2.11786755518534</t>
         </is>
       </c>
     </row>
@@ -639,17 +639,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0.448493342676944</t>
+          <t>2.23032943098285</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>-105.703703703704</t>
+          <t>5.18858808829654</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>70.2962962962963</t>
+          <t>-0.655619682275242</t>
         </is>
       </c>
     </row>
@@ -661,17 +661,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.40276903713027</t>
+          <t>0.821201679092788</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>-93.0617283950617</t>
+          <t>2.84899149164039</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>117.703703703704</t>
+          <t>-2.84899149164039</t>
         </is>
       </c>
     </row>
@@ -683,17 +683,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.404487280771054</t>
+          <t>1.4188045290208</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>-156.271604938272</t>
+          <t>6.35838638662462</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>105.061728395062</t>
+          <t>-1.17785106545742</t>
         </is>
       </c>
     </row>
@@ -705,17 +705,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0.375641966250917</t>
+          <t>0.725683241634658</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>-139.415637860082</t>
+          <t>3.68456170473187</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>168.271604938272</t>
+          <t>-3.68456170473187</t>
         </is>
       </c>
     </row>
@@ -727,17 +727,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0.376761470252768</t>
+          <t>1.0761755994228</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>-223.695473251029</t>
+          <t>7.69529872757099</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>151.415637860082</t>
+          <t>-1.77468693195134</t>
         </is>
       </c>
     </row>
@@ -749,17 +749,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>0.357579355379404</t>
+          <t>0.65864861193663</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>-201.22085048011</t>
+          <t>4.63949909112214</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>235.695473251029</t>
+          <t>-4.63949909112214</t>
         </is>
       </c>
     </row>
@@ -771,17 +771,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>0.358339530204278</t>
+          <t>0.888443216727787</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>-313.593964334705</t>
+          <t>9.22319854579542</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>213.22085048011</t>
+          <t>-2.45678506508724</t>
         </is>
       </c>
     </row>
@@ -793,17 +793,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>0.345132668795659</t>
+          <t>0.609392798945553</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>-283.627800640146</t>
+          <t>5.73085610413959</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>325.593964334705</t>
+          <t>-5.73085610413959</t>
         </is>
       </c>
     </row>
@@ -815,17 +815,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>0.345663488661081</t>
+          <t>0.770790853071912</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>-433.45861911294</t>
+          <t>10.9693697666233</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>295.627800640146</t>
+          <t>-3.23632578867113</t>
         </is>
       </c>
     </row>
@@ -837,17 +837,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>0.336351822692662</t>
+          <t>0.571966057190265</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>-393.503734186862</t>
+          <t>6.97812126187381</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>445.45861911294</t>
+          <t>-6.97812126187381</t>
         </is>
       </c>
     </row>
@@ -859,17 +859,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>0.336729781235597</t>
+          <t>0.69075194580724</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>-593.278158817253</t>
+          <t>12.9649940189981</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>405.503734186862</t>
+          <t>-4.12722947276701</t>
         </is>
       </c>
     </row>
@@ -881,17 +881,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>0.330053912767581</t>
+          <t>0.542796502683056</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>-540.004978915816</t>
+          <t>8.40356715642721</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>605.278158817253</t>
+          <t>-8.40356715642721</t>
         </is>
       </c>
     </row>
@@ -903,17 +903,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>0.330326784652879</t>
+          <t>0.633217788287162</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>-806.370878423004</t>
+          <t>15.2457074502835</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>552.004978915816</t>
+          <t>-5.14540511173372</t>
         </is>
       </c>
     </row>
@@ -925,17 +925,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>0.325483111056535</t>
+          <t>0.519609496776617</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>-735.339971887754</t>
+          <t>10.032648178774</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>818.370878423004</t>
+          <t>-10.032648178774</t>
         </is>
       </c>
     </row>
@@ -947,17 +947,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>0.325682093022786</t>
+          <t>0.590203432311191</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>-1090.49450456401</t>
+          <t>17.8522370860383</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>747.339971887754</t>
+          <t>-6.30903441340997</t>
         </is>
       </c>
     </row>
@@ -969,17 +969,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>0.322137236245637</t>
+          <t>0.500887345725371</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>-995.786629183672</t>
+          <t>11.894455061456</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1102.49450456401</t>
+          <t>-11.894455061456</t>
         </is>
       </c>
     </row>
@@ -991,17 +991,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>0.322283397245039</t>
+          <t>0.557090753137568</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>-1469.32600608534</t>
+          <t>20.8311280983295</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1007.78662918367</t>
+          <t>-7.63889647246854</t>
         </is>
       </c>
     </row>
@@ -1013,17 +1013,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>0.319672627737818</t>
+          <t>0.485578372856879</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>-1343.04883891156</t>
+          <t>14.0222343559497</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1481.32600608534</t>
+          <t>-14.0222343559497</t>
         </is>
       </c>
     </row>
@@ -1035,17 +1035,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>0.319780565006081</t>
+          <t>0.531022406342188</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>-1974.43467478045</t>
+          <t>24.2355749695195</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1355.04883891156</t>
+          <t>-9.15873882567833</t>
         </is>
       </c>
     </row>
@@ -1057,17 +1057,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>0.31784877896308</t>
+          <t>0.472930673630806</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>-1806.06511854875</t>
+          <t>16.4539821210853</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1986.43467478045</t>
+          <t>-16.4539821210853</t>
         </is>
       </c>
     </row>
@@ -1079,17 +1079,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>0.31792880394653</t>
+          <t>0.51013517563245</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>-2647.91289970727</t>
+          <t>28.1263713937365</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1818.06511854875</t>
+          <t>-10.8957015150609</t>
         </is>
       </c>
     </row>
@@ -1101,17 +1101,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>0.316494491699773</t>
+          <t>0.462392365292517</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>-2423.420158065</t>
+          <t>19.2331224240975</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2659.91289970727</t>
+          <t>-19.2331224240975</t>
         </is>
       </c>
     </row>
@@ -1123,17 +1123,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>0.316553996279098</t>
+          <t>0.493161902885715</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>-3545.88386627636</t>
+          <t>32.572995878556</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2435.420158065</t>
+          <t>-12.8808017314982</t>
         </is>
       </c>
     </row>
@@ -1145,17 +1145,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>0.315486325692277</t>
+          <t>0.453549237264532</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>-3246.56021075333</t>
+          <t>22.4092827703972</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>3557.88386627636</t>
+          <t>-22.4092827703971</t>
         </is>
       </c>
     </row>
@@ -1167,17 +1167,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>0.315530668155383</t>
+          <t>0.479210599348736</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>-4743.17848836848</t>
+          <t>37.6548524326354</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>3258.56021075333</t>
+          <t>-15.1494876931408</t>
         </is>
       </c>
     </row>
@@ -1189,17 +1189,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>0.314734406137643</t>
+          <t>0.446084399960319</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>-4344.08028100444</t>
+          <t>26.0391803090253</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>4755.17848836848</t>
+          <t>-26.0391803090253</t>
         </is>
       </c>
     </row>
@@ -1211,17 +1211,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>0.314767503476076</t>
+          <t>0.467635082120224</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>-6339.57131782464</t>
+          <t>43.4626884944405</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>4356.08028100444</t>
+          <t>-17.7422716493038</t>
         </is>
       </c>
     </row>
@@ -1233,17 +1233,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>0.314172814405812</t>
+          <t>0.439751375500424</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>-5807.44037467259</t>
+          <t>30.1876346388861</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>6351.57131782464</t>
+          <t>-30.1876346388861</t>
         </is>
       </c>
     </row>
@@ -1255,17 +1255,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>0.314197548249811</t>
+          <t>0.457955746335588</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>-8468.09509043286</t>
+          <t>50.1002154222177</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>5819.44037467259</t>
+          <t>-20.7054533134901</t>
         </is>
       </c>
     </row>
@@ -1277,17 +1277,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>0.313752934063438</t>
+          <t>0.434355676871654</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>-7758.58716623012</t>
+          <t>34.9287253015841</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>8480.09509043286</t>
+          <t>-34.9287253015841</t>
         </is>
       </c>
     </row>
@@ -1299,17 +1299,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>0.313771434530189</t>
+          <t>0.449809175561137</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>-11306.1267872438</t>
+          <t>57.6859604825345</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>7770.58716623012</t>
+          <t>-24.0919466439886</t>
         </is>
       </c>
     </row>
@@ -1321,17 +1321,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>0.31343875958449</t>
+          <t>0.429741903751808</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>-10360.1162216402</t>
+          <t>40.3471146303818</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>11318.1267872438</t>
+          <t>-40.3471146303818</t>
         </is>
       </c>
     </row>
@@ -1343,17 +1343,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>0.31345260695574</t>
+          <t>0.442915040249126</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>-15090.1690496584</t>
+          <t>66.3553834086108</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>10372.1162216402</t>
+          <t>-27.962224735987</t>
         </is>
       </c>
     </row>
@@ -1365,17 +1365,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>0.313203541323439</t>
+          <t>0.425784515601177</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>-13828.8216288535</t>
+          <t>46.5395595775792</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>15102.1690496584</t>
+          <t>-46.5395595775792</t>
         </is>
       </c>
     </row>
@@ -1387,17 +1387,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>0.313213911155419</t>
+          <t>0.437053734435276</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>-20135.5587328779</t>
+          <t>76.2632953241267</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>13840.8216288535</t>
+          <t>-32.3853996982709</t>
         </is>
       </c>
     </row>
@@ -1409,17 +1409,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>0.3130273591774</t>
+          <t>0.422381111737043</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>-18453.7621718047</t>
+          <t>53.6166395172334</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>20147.5587328779</t>
+          <t>-53.6166395172333</t>
         </is>
       </c>
     </row>
@@ -1431,17 +1431,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>0.313035127739634</t>
+          <t>0.432050891004709</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>-26862.7449771705</t>
+          <t>87.5866232275734</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>18465.7621718047</t>
+          <t>-37.4404567980238</t>
         </is>
       </c>
     </row>
@@ -1453,17 +1453,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>0.312895352588797</t>
+          <t>0.419447455372509</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>-24620.3495624063</t>
+          <t>61.7047308768381</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>26874.7449771705</t>
+          <t>-61.7047308768381</t>
         </is>
       </c>
     </row>
@@ -1475,17 +1475,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>0.312901174061231</t>
+          <t>0.4277664238094</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>-35832.3266362273</t>
+          <t>100.527569402941</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>24632.3495624063</t>
+          <t>-43.2176649120272</t>
         </is>
       </c>
     </row>
@@ -1497,17 +1497,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>0.312796420689049</t>
+          <t>0.41691373311658</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>-32842.4660832084</t>
+          <t>70.9482638592436</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>35844.3266362273</t>
+          <t>-70.9482638592435</t>
         </is>
       </c>
     </row>
@@ -1519,17 +1519,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>0.312800784012528</t>
+          <t>0.424086621043218</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>-47791.7688483031</t>
+          <t>115.31722217479</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>32854.4660832084</t>
+          <t>-49.8201884708883</t>
         </is>
       </c>
     </row>
@@ -1541,17 +1541,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>0.31272226281015</t>
+          <t>0.414721704296541</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>-43805.2881109445</t>
+          <t>81.5123015534212</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>47803.7688483031</t>
+          <t>-81.5123015534212</t>
         </is>
       </c>
     </row>
@@ -1563,17 +1563,17 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>0.312725533739841</t>
+          <t>0.420918339625499</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>-63737.6917977375</t>
+          <t>132.219682485474</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>43817.2881109445</t>
+          <t>-57.3659296810152</t>
         </is>
       </c>
     </row>
@@ -1585,17 +1585,17 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>0.312666667472428</t>
+          <t>0.412822500926044</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>-58422.3841479261</t>
+          <t>93.5854874896242</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>63749.6917977375</t>
+          <t>-93.5854874896242</t>
         </is>
       </c>
     </row>
@@ -1607,17 +1607,17 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>0.312669119791106</t>
+          <t>0.418184674299507</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>-84998.9223969833</t>
+          <t>151.536779983399</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>58434.3841479261</t>
+          <t>-65.9896339211602</t>
         </is>
       </c>
     </row>
@@ -1629,17 +1629,17 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>0.312624983939715</t>
+          <t>0.411174910093095</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>-77911.8455305681</t>
+          <t>107.383414273856</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>85010.9223969833</t>
+          <t>-107.383414273856</t>
         </is>
       </c>
     </row>
@@ -1651,17 +1651,17 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>0.312626822684749</t>
+          <t>0.41582167998165</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>-113347.229862644</t>
+          <t>173.61346283817</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>77923.8455305681</t>
+          <t>-75.8452959098973</t>
         </is>
       </c>
     </row>
@@ -1673,17 +1673,17 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>0.312593728583132</t>
+          <t>0.409744018665044</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>-103897.794040757</t>
+          <t>123.152473455836</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>113359.229862644</t>
+          <t>-123.152473455836</t>
         </is>
       </c>
     </row>
@@ -1695,17 +1695,17 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>0.312595107364144</t>
+          <t>0.41377585835197</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>-151144.973150193</t>
+          <t>198.843957529337</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>103909.794040757</t>
+          <t>-87.1089096113112</t>
         </is>
       </c>
     </row>
@@ -1717,17 +1717,17 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>0.312570291166716</t>
+          <t>0.408500133376203</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>-138545.725387677</t>
+          <t>141.174255378098</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>151156.973150193</t>
+          <t>-141.174255378098</t>
         </is>
       </c>
     </row>
@@ -1739,17 +1739,17 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>0.312571325096275</t>
+          <t>0.412002207087739</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>-201541.964200257</t>
+          <t>227.678808604957</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>138557.725387677</t>
+          <t>-99.9816109843557</t>
         </is>
       </c>
     </row>
@@ -1761,17 +1761,17 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>0.312552715410695</t>
+          <t>0.407417912564748</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>-184742.967183569</t>
+          <t>161.770577574969</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>201553.964200257</t>
+          <t>-161.770577574969</t>
         </is>
       </c>
     </row>
@@ -1783,17 +1783,17 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>0.312553490770018</t>
+          <t>0.410462688902116</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>-268737.952267009</t>
+          <t>260.63292411995</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>184754.967183569</t>
+          <t>-114.693269696406</t>
         </is>
       </c>
     </row>
@@ -1805,17 +1805,17 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>0.312539534890743</t>
+          <t>0.406475662276478</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>-246339.289578092</t>
+          <t>185.30923151425</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>268749.952267009</t>
+          <t>-185.30923151425</t>
         </is>
       </c>
     </row>
@@ -1827,17 +1827,17 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>0.31254011636083</t>
+          <t>0.409125017720091</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>-358332.603022679</t>
+          <t>298.294770422801</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>246351.289578092</t>
+          <t>-131.50659393875</t>
         </is>
       </c>
     </row>
@@ -1849,17 +1849,17 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>0.312529650230282</t>
+          <t>0.405654761265602</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>-328467.719437455</t>
+          <t>212.210550302</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>358344.603022679</t>
+          <t>-212.210550302</t>
         </is>
       </c>
     </row>
@@ -1871,17 +1871,17 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>0.31253008630506</t>
+          <t>0.407961687212301</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>-477792.137363571</t>
+          <t>341.336880483201</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>328479.719437455</t>
+          <t>-150.721821644286</t>
         </is>
       </c>
     </row>
@@ -1893,17 +1893,17 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>0.312522237145242</t>
+          <t>0.404939188004586</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>-437972.292583274</t>
+          <t>242.954914630858</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>477804.137363571</t>
+          <t>-242.954914630858</t>
         </is>
       </c>
     </row>
@@ -1915,17 +1915,17 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>0.312522564185696</t>
+          <t>0.406949186545246</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>-637071.516484762</t>
+          <t>390.527863409372</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>437984.292583274</t>
+          <t>-172.682081879184</t>
         </is>
       </c>
     </row>
@@ -1937,17 +1937,17 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>0.312516677562243</t>
+          <t>0.404315129118394</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>-583978.390111032</t>
+          <t>278.091331006694</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>637083.516484762</t>
+          <t>-278.091331006694</t>
         </is>
       </c>
     </row>
@@ -1959,17 +1959,17 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>0.312516922833792</t>
+          <t>0.406067362217127</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>-849444.021979682</t>
+          <t>446.746129610711</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>583990.390111032</t>
+          <t>-197.779522147639</t>
         </is>
       </c>
     </row>
@@ -1981,17 +1981,17 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>0.3125125080048</t>
+          <t>0.403770653336093</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>-778653.186814709</t>
+          <t>318.247235436222</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>849456.021979682</t>
+          <t>-318.247235436222</t>
         </is>
       </c>
     </row>
@@ -2003,17 +2003,17 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>0.312512691953517</t>
+          <t>0.405298894966513</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>-1132607.36263958</t>
+          <t>510.995576697955</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>778665.186814709</t>
+          <t>-226.462311025873</t>
         </is>
       </c>
     </row>
@@ -2025,17 +2025,17 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>0.31250938090973</t>
+          <t>0.403295438557709</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>-1038219.58241961</t>
+          <t>364.139697641397</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>1132619.36263958</t>
+          <t>-364.139697641397</t>
         </is>
       </c>
     </row>
@@ -2047,17 +2047,17 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>0.312509518868487</t>
+          <t>0.404628868131311</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>-1510158.48351944</t>
+          <t>584.423516226235</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>1038231.58241961</t>
+          <t>-259.242641172426</t>
         </is>
       </c>
     </row>
@@ -2069,17 +2069,17 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>0.312507035629497</t>
+          <t>0.402880542284835</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>-1384308.10989282</t>
+          <t>416.588225875882</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>1510170.48351944</t>
+          <t>-416.588225875882</t>
         </is>
       </c>
     </row>
@@ -2091,17 +2091,17 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>0.312507139097001</t>
+          <t>0.404044409290748</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>-2013559.97802591</t>
+          <t>668.341161401411</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>1384320.10989282</t>
+          <t>-296.70587562563</t>
         </is>
       </c>
     </row>
@@ -2113,17 +2113,17 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>0.312505276692423</t>
+          <t>0.402518207685568</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>-1845759.47985709</t>
+          <t>476.529401001008</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2013571.97802591</t>
+          <t>-476.529401001008</t>
         </is>
       </c>
     </row>
@@ -2135,17 +2135,17 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>0.312505354292171</t>
+          <t>0.403534391090603</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>-2684761.97070122</t>
+          <t>764.247041601613</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>1845771.47985709</t>
+          <t>-339.521000715006</t>
         </is>
       </c>
     </row>
@@ -2157,17 +2157,17 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>0.312503957502611</t>
+          <t>0.402201699119983</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>-2461027.97314278</t>
+          <t>545.033601144009</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2684773.97070122</t>
+          <t>-545.033601144009</t>
         </is>
       </c>
     </row>
@@ -2179,17 +2179,17 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>0.312504015701927</t>
+          <t>0.403089180213333</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>-3579697.96093496</t>
+          <t>873.853761830414</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2461039.97314278</t>
+          <t>-388.452572245721</t>
         </is>
       </c>
     </row>
@@ -2201,17 +2201,17 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>0.312502968117561</t>
+          <t>0.401925162158787</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>-3281385.96419038</t>
+          <t>623.324115593153</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>3579709.96093496</t>
+          <t>-623.324115593153</t>
         </is>
       </c>
     </row>
@@ -2223,17 +2223,17 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>0.31250301176677</t>
+          <t>0.402700425779826</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>-4772945.94791328</t>
+          <t>999.118584949044</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>3281397.96419038</t>
+          <t>-444.374368280824</t>
         </is>
       </c>
     </row>
@@ -2245,17 +2245,17 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>0.312502226082885</t>
+          <t>0.40168350407071</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>-4375196.6189205</t>
+          <t>712.798989249318</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>4772957.94791328</t>
+          <t>-712.798989249317</t>
         </is>
       </c>
     </row>
@@ -2267,17 +2267,17 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>0.312502258819635</t>
+          <t>0.402360880250507</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>-6363943.26388437</t>
+          <t>1142.27838279891</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>4375208.6189205</t>
+          <t>-508.284992320941</t>
         </is>
       </c>
     </row>
@@ -2289,17 +2289,17 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>0.31250166955919</t>
+          <t>0.401472291496644</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>-5833610.82522734</t>
+          <t>815.055987713506</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>6363955.26388437</t>
+          <t>-815.055987713505</t>
         </is>
       </c>
     </row>
@@ -2311,17 +2311,17 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>0.312501694111665</t>
+          <t>0.402064247269003</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>-8485273.01851249</t>
+          <t>1305.88958034161</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>5833622.82522734</t>
+          <t>-581.325705509647</t>
         </is>
       </c>
     </row>
@@ -2333,17 +2333,17 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>0.31250125216772</t>
+          <t>0.401287662617463</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>-7778163.10030312</t>
+          <t>931.921128815435</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>8485285.01851249</t>
+          <t>-931.921128815435</t>
         </is>
       </c>
     </row>
@@ -2355,17 +2355,17 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>0.312501270582026</t>
+          <t>0.401805051962382</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>-11313712.69135</t>
+          <t>1492.8738061047</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>7778175.10030312</t>
+          <t>-664.800806296739</t>
         </is>
       </c>
     </row>
@@ -2377,17 +2377,17 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>0.31250093912485</t>
+          <t>0.401126251592756</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>-10370899.4670708</t>
+          <t>1065.48129007478</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>11313724.69135</t>
+          <t>-1065.48129007478</t>
         </is>
       </c>
     </row>
@@ -2399,17 +2399,17 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>0.312500952935551</t>
+          <t>0.401578530051845</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>-15084965.5884666</t>
+          <t>1706.57006411965</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>10370911.4670708</t>
+          <t>-760.200921481988</t>
         </is>
       </c>
     </row>
@@ -2421,17 +2421,17 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>0.312500704343108</t>
+          <t>0.400985123425903</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>-13827881.2894278</t>
+          <t>1218.12147437118</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>15084977.5884666</t>
+          <t>-1218.12147437118</t>
         </is>
       </c>
     </row>
@@ -2443,17 +2443,17 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>0.312500714701118</t>
+          <t>0.401380532791458</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>-20113302.7846222</t>
+          <t>1950.79435899389</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>13827893.2894278</t>
+          <t>-869.229624550843</t>
         </is>
       </c>
     </row>
@@ -2465,17 +2465,17 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>0.312500528257033</t>
+          <t>0.400861717716944</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>-18437190.3859037</t>
+          <t>1392.56739928135</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>20113314.7846222</t>
+          <t>-1392.56739928135</t>
         </is>
       </c>
     </row>
@@ -2487,17 +2487,17 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>0.312500536025532</t>
+          <t>0.401207445280712</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>-26817752.3794963</t>
+          <t>2229.90783885016</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>18437202.3859037</t>
+          <t>-993.833856629535</t>
         </is>
       </c>
     </row>
@@ -2509,17 +2509,17 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>0.312500396192607</t>
+          <t>0.400753800013942</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>-24582935.8478716</t>
+          <t>1591.93417060726</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>26817764.3794963</t>
+          <t>-1591.93417060725</t>
         </is>
       </c>
     </row>
@@ -2531,17 +2531,17 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>0.312500402018977</t>
+          <t>0.401056116119865</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>-35757018.505995</t>
+          <t>2548.89467297161</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>24582947.8478716</t>
+          <t>-1136.2386932909</t>
         </is>
       </c>
     </row>
@@ -2553,17 +2553,17 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>0.312500297144361</t>
+          <t>0.400659419677649</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>-32777263.1304954</t>
+          <t>1819.78190926543</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>35757030.505995</t>
+          <t>-1819.78190926543</t>
         </is>
       </c>
     </row>
@@ -2575,17 +2575,17 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>0.312500301514136</t>
+          <t>0.400923796718443</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>-47676040.0079933</t>
+          <t>2913.45105482469</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>32777275.1304954</t>
+          <t>-1298.98707804674</t>
         </is>
       </c>
     </row>
@@ -2597,17 +2597,17 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>0.312500222858218</t>
+          <t>0.400576873342432</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>-43703032.8406606</t>
+          <t>2080.17932487478</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>47676052.0079933</t>
+          <t>-2080.17932487478</t>
         </is>
       </c>
     </row>
@@ -2619,17 +2619,17 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>0.312500226135547</t>
+          <t>0.400808088844318</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>-63568068.6773245</t>
+          <t>3330.08691979965</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>43703044.8406606</t>
+          <t>-1484.98523205342</t>
         </is>
       </c>
     </row>
@@ -2641,17 +2641,17 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>0.312500167143634</t>
+          <t>0.400504673195718</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>-58270725.7875474</t>
+          <t>2377.77637128547</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>63568080.6773245</t>
+          <t>-2377.77637128546</t>
         </is>
       </c>
     </row>

</xml_diff>